<commit_message>
remove personal Bmap key
</commit_message>
<xml_diff>
--- a/dir/crawl_recorder.xlsx
+++ b/dir/crawl_recorder.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20191\Desktop\github\streetview_images_crawler\dir\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85EB0D29-FAA2-4784-82ED-425372711CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -169,12 +163,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -182,15 +176,8 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -236,23 +223,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -294,7 +273,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,27 +305,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -378,24 +339,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -571,14 +514,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -615,10 +558,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>113.93381534248461</v>
+        <v>113.9338153424846</v>
       </c>
       <c r="D2">
-        <v>22.528024513977719</v>
+        <v>22.52802451397772</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -636,7 +579,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -644,10 +587,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>113.93381534248461</v>
+        <v>113.9338153424846</v>
       </c>
       <c r="D3">
-        <v>22.528024513977719</v>
+        <v>22.52802451397772</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -665,7 +608,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -673,10 +616,10 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>113.93381534248461</v>
+        <v>113.9338153424846</v>
       </c>
       <c r="D4">
-        <v>22.528024513977719</v>
+        <v>22.52802451397772</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -688,13 +631,13 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -702,10 +645,10 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>113.93381534248461</v>
+        <v>113.9338153424846</v>
       </c>
       <c r="D5">
-        <v>22.528024513977719</v>
+        <v>22.52802451397772</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -723,7 +666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -734,7 +677,7 @@
         <v>113.9333821902438</v>
       </c>
       <c r="D6">
-        <v>22.528032224229261</v>
+        <v>22.52803222422926</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -752,7 +695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -763,7 +706,7 @@
         <v>113.9333821902438</v>
       </c>
       <c r="D7">
-        <v>22.528032224229261</v>
+        <v>22.52803222422926</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
@@ -781,7 +724,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -792,7 +735,7 @@
         <v>113.9333821902438</v>
       </c>
       <c r="D8">
-        <v>22.528032224229261</v>
+        <v>22.52803222422926</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
@@ -810,7 +753,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -821,7 +764,7 @@
         <v>113.9333821902438</v>
       </c>
       <c r="D9">
-        <v>22.528032224229261</v>
+        <v>22.52803222422926</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
@@ -839,7 +782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -850,7 +793,7 @@
         <v>113.9329490300419</v>
       </c>
       <c r="D10">
-        <v>22.528039548211861</v>
+        <v>22.52803954821186</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
@@ -868,7 +811,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>0</v>
       </c>
@@ -879,7 +822,7 @@
         <v>113.9329490300419</v>
       </c>
       <c r="D11">
-        <v>22.528039548211861</v>
+        <v>22.52803954821186</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -897,7 +840,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -908,7 +851,7 @@
         <v>113.9329490300419</v>
       </c>
       <c r="D12">
-        <v>22.528039548211861</v>
+        <v>22.52803954821186</v>
       </c>
       <c r="F12" t="s">
         <v>9</v>
@@ -926,7 +869,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>0</v>
       </c>
@@ -937,7 +880,7 @@
         <v>113.9329490300419</v>
       </c>
       <c r="D13">
-        <v>22.528039548211861</v>
+        <v>22.52803954821186</v>
       </c>
       <c r="F13" t="s">
         <v>9</v>
@@ -955,7 +898,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -966,7 +909,7 @@
         <v>113.9325158696837</v>
       </c>
       <c r="D14">
-        <v>22.528046864306951</v>
+        <v>22.52804686430695</v>
       </c>
       <c r="F14" t="s">
         <v>9</v>
@@ -984,7 +927,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -995,7 +938,7 @@
         <v>113.9325158696837</v>
       </c>
       <c r="D15">
-        <v>22.528046864306951</v>
+        <v>22.52804686430695</v>
       </c>
       <c r="F15" t="s">
         <v>9</v>
@@ -1013,7 +956,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>0</v>
       </c>
@@ -1024,7 +967,7 @@
         <v>113.9325158696837</v>
       </c>
       <c r="D16">
-        <v>22.528046864306951</v>
+        <v>22.52804686430695</v>
       </c>
       <c r="F16" t="s">
         <v>9</v>
@@ -1042,7 +985,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>0</v>
       </c>
@@ -1053,7 +996,7 @@
         <v>113.9325158696837</v>
       </c>
       <c r="D17">
-        <v>22.528046864306951</v>
+        <v>22.52804686430695</v>
       </c>
       <c r="F17" t="s">
         <v>9</v>
@@ -1071,7 +1014,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -1082,7 +1025,7 @@
         <v>113.9320827093254</v>
       </c>
       <c r="D18">
-        <v>22.528054180395301</v>
+        <v>22.5280541803953</v>
       </c>
       <c r="F18" t="s">
         <v>9</v>
@@ -1100,7 +1043,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>0</v>
       </c>
@@ -1111,7 +1054,7 @@
         <v>113.9320827093254</v>
       </c>
       <c r="D19">
-        <v>22.528054180395301</v>
+        <v>22.5280541803953</v>
       </c>
       <c r="F19" t="s">
         <v>9</v>
@@ -1129,7 +1072,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>0</v>
       </c>
@@ -1140,7 +1083,7 @@
         <v>113.9320827093254</v>
       </c>
       <c r="D20">
-        <v>22.528054180395301</v>
+        <v>22.5280541803953</v>
       </c>
       <c r="F20" t="s">
         <v>9</v>
@@ -1152,13 +1095,13 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>0</v>
       </c>
@@ -1169,7 +1112,7 @@
         <v>113.9320827093254</v>
       </c>
       <c r="D21">
-        <v>22.528054180395301</v>
+        <v>22.5280541803953</v>
       </c>
       <c r="F21" t="s">
         <v>9</v>
@@ -1187,7 +1130,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>0</v>
       </c>
@@ -1198,7 +1141,7 @@
         <v>113.9316495489757</v>
       </c>
       <c r="D22">
-        <v>22.528061496918209</v>
+        <v>22.52806149691821</v>
       </c>
       <c r="F22" t="s">
         <v>9</v>
@@ -1216,7 +1159,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>0</v>
       </c>
@@ -1227,7 +1170,7 @@
         <v>113.9316495489757</v>
       </c>
       <c r="D23">
-        <v>22.528061496918209</v>
+        <v>22.52806149691821</v>
       </c>
       <c r="F23" t="s">
         <v>9</v>
@@ -1245,7 +1188,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -1256,7 +1199,7 @@
         <v>113.9316495489757</v>
       </c>
       <c r="D24">
-        <v>22.528061496918209</v>
+        <v>22.52806149691821</v>
       </c>
       <c r="F24" t="s">
         <v>9</v>
@@ -1274,7 +1217,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>0</v>
       </c>
@@ -1285,7 +1228,7 @@
         <v>113.9316495489757</v>
       </c>
       <c r="D25">
-        <v>22.528061496918209</v>
+        <v>22.52806149691821</v>
       </c>
       <c r="F25" t="s">
         <v>9</v>
@@ -1303,7 +1246,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>0</v>
       </c>
@@ -1332,7 +1275,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>0</v>
       </c>
@@ -1361,7 +1304,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>0</v>
       </c>
@@ -1390,7 +1333,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>0</v>
       </c>
@@ -1419,7 +1362,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>0</v>
       </c>
@@ -1430,7 +1373,7 @@
         <v>113.9307832286713</v>
       </c>
       <c r="D30">
-        <v>22.528076149574659</v>
+        <v>22.52807614957466</v>
       </c>
       <c r="F30" t="s">
         <v>9</v>
@@ -1448,7 +1391,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>0</v>
       </c>
@@ -1459,7 +1402,7 @@
         <v>113.9307832286713</v>
       </c>
       <c r="D31">
-        <v>22.528076149574659</v>
+        <v>22.52807614957466</v>
       </c>
       <c r="F31" t="s">
         <v>9</v>
@@ -1477,7 +1420,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>0</v>
       </c>
@@ -1488,7 +1431,7 @@
         <v>113.9307832286713</v>
       </c>
       <c r="D32">
-        <v>22.528076149574659</v>
+        <v>22.52807614957466</v>
       </c>
       <c r="F32" t="s">
         <v>9</v>
@@ -1506,7 +1449,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -1517,7 +1460,7 @@
         <v>113.9307832286713</v>
       </c>
       <c r="D33">
-        <v>22.528076149574659</v>
+        <v>22.52807614957466</v>
       </c>
       <c r="F33" t="s">
         <v>9</v>
@@ -1536,8 +1479,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>